<commit_message>
Updated Task Asgmt List 11Dec17
Added Site & App Rebuild tasks
</commit_message>
<xml_diff>
--- a/Task Assignment List.xlsx
+++ b/Task Assignment List.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="165" windowWidth="16275" windowHeight="7680"/>
+    <workbookView xWindow="360" yWindow="165" windowWidth="16275" windowHeight="7680" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Planning Tasks" sheetId="1" r:id="rId1"/>
+    <sheet name="Rebuild Tasks" sheetId="4" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="54">
   <si>
     <t>Task</t>
   </si>
@@ -150,6 +150,100 @@
       </rPr>
       <t>:  For each of the following tasks, please provide your inputs on the Smithgall Woods Project Charter document in GitHub by the due date.</t>
     </r>
+  </si>
+  <si>
+    <t>https://demo.bpmn.io/</t>
+  </si>
+  <si>
+    <t>http://alexdp.free.fr/violetumleditor/page.php</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Instruction</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>:  Before you begin working on your assigned task, please watch the tutorials on WordPress &amp; PHP.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve"> -- Create User Account / Login</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -- View FAQs</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -- Edit Profile / Password / Interest</t>
+  </si>
+  <si>
+    <t>Volunteer Hours Database</t>
+  </si>
+  <si>
+    <t>Home Page &amp; Search Feature</t>
+  </si>
+  <si>
+    <t>About Us Friends &amp; Activities</t>
+  </si>
+  <si>
+    <t>Events &amp; Volunteer Opportunities</t>
+  </si>
+  <si>
+    <t>Friends Corner, Visitors &amp; Contact Us</t>
+  </si>
+  <si>
+    <t>Choose a theme for all site pages</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -- Add &amp; View Volunteer Hours</t>
+  </si>
+  <si>
+    <t>DB must be created before building the app use cases</t>
+  </si>
+  <si>
+    <t>First Iteration Due Date</t>
+  </si>
+  <si>
+    <t>Final Iteration Due Date</t>
+  </si>
+  <si>
+    <t>Volunteer Hours App:</t>
+  </si>
+  <si>
+    <t>Site &amp; App Rebuild Task</t>
+  </si>
+  <si>
+    <t>Volunteer Reports App:</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -- Select by Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -- Select by Activity</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -- Select by Location</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -- Select by Project</t>
   </si>
 </sst>
 </file>
@@ -204,7 +298,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -220,6 +314,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -246,7 +346,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -260,11 +360,23 @@
     <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -598,9 +710,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I17" sqref="I17"/>
+      <selection pane="bottomLeft" activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -612,12 +724,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
     </row>
     <row r="2" spans="1:4" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
@@ -656,6 +768,9 @@
       </c>
       <c r="C4" s="6">
         <v>43009</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
@@ -765,6 +880,9 @@
       <c r="C16" s="6">
         <v>43016</v>
       </c>
+      <c r="D16" s="5" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="17" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
@@ -772,12 +890,12 @@
       <c r="C17" s="6"/>
     </row>
     <row r="18" spans="1:4" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="8" t="s">
+      <c r="A18" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B18" s="8"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="8"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
     </row>
     <row r="19" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
@@ -878,21 +996,277 @@
   <hyperlinks>
     <hyperlink ref="D3" r:id="rId1"/>
     <hyperlink ref="D13" r:id="rId2"/>
+    <hyperlink ref="D16" r:id="rId3"/>
+    <hyperlink ref="D4" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I5" sqref="I5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="47.85546875" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" customWidth="1"/>
+    <col min="3" max="4" width="13.42578125" customWidth="1"/>
+    <col min="5" max="5" width="40.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+    </row>
+    <row r="2" spans="1:5" ht="55.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="6">
+        <v>43119</v>
+      </c>
+      <c r="D3" s="6">
+        <v>43147</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" s="3"/>
+      <c r="C4" s="6">
+        <v>43119</v>
+      </c>
+      <c r="D4" s="6">
+        <v>43147</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B5" s="3"/>
+      <c r="C5" s="6">
+        <v>43119</v>
+      </c>
+      <c r="D5" s="6">
+        <v>43147</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B6" s="3"/>
+      <c r="C6" s="6">
+        <v>43119</v>
+      </c>
+      <c r="D6" s="6">
+        <v>43147</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B7" s="10"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="3"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+    </row>
+    <row r="9" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" s="3"/>
+      <c r="C9" s="6">
+        <v>43119</v>
+      </c>
+      <c r="D9" s="6">
+        <v>43147</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B10" s="3"/>
+      <c r="C10" s="6">
+        <v>43119</v>
+      </c>
+      <c r="D10" s="6">
+        <v>43147</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" s="3"/>
+      <c r="C11" s="6">
+        <v>43119</v>
+      </c>
+      <c r="D11" s="6">
+        <v>43147</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" s="3"/>
+      <c r="C12" s="6">
+        <v>43119</v>
+      </c>
+      <c r="D12" s="6">
+        <v>43147</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="37.5" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13" s="2"/>
+      <c r="C13" s="6">
+        <v>43089</v>
+      </c>
+      <c r="D13" s="6"/>
+      <c r="E13" s="9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B14" s="10"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
+    </row>
+    <row r="15" spans="1:5" ht="18.75" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="1"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+    </row>
+    <row r="16" spans="1:5" ht="18.75" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="1"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+    </row>
+    <row r="17" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B17" s="3"/>
+      <c r="C17" s="6">
+        <v>43119</v>
+      </c>
+      <c r="D17" s="6">
+        <v>43147</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B18" s="3"/>
+      <c r="C18" s="6">
+        <v>43119</v>
+      </c>
+      <c r="D18" s="6">
+        <v>43147</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B19" s="3"/>
+      <c r="C19" s="6">
+        <v>43119</v>
+      </c>
+      <c r="D19" s="6">
+        <v>43147</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B20" s="3"/>
+      <c r="C20" s="6">
+        <v>43119</v>
+      </c>
+      <c r="D20" s="6">
+        <v>43147</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A21" s="1"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+    </row>
+    <row r="22" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B22" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:E1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Updated Task Asgmt List 12Dec17
Added Home Page to app and Follow-up Schedule
</commit_message>
<xml_diff>
--- a/Task Assignment List.xlsx
+++ b/Task Assignment List.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="55">
   <si>
     <t>Task</t>
   </si>
@@ -186,12 +186,6 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve"> -- Create User Account / Login</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> -- View FAQs</t>
-  </si>
-  <si>
     <t xml:space="preserve"> -- Edit Profile / Password / Interest</t>
   </si>
   <si>
@@ -244,13 +238,22 @@
   </si>
   <si>
     <t xml:space="preserve"> -- Select by Project</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -- Home Page &amp; View FAQs</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -- Create User Account / Login / Logout</t>
+  </si>
+  <si>
+    <t>Rebuild Task Update Schedule:</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -292,6 +295,14 @@
       <b/>
       <u/>
       <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -346,7 +357,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -360,12 +371,6 @@
     <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -378,6 +383,16 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -724,12 +739,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
     </row>
     <row r="2" spans="1:4" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
@@ -890,12 +905,12 @@
       <c r="C17" s="6"/>
     </row>
     <row r="18" spans="1:4" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="7" t="s">
+      <c r="A18" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="B18" s="7"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
+      <c r="B18" s="11"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="11"/>
     </row>
     <row r="19" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
@@ -1006,11 +1021,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I5" sqref="I5"/>
+      <selection pane="bottomLeft" activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1019,37 +1034,39 @@
     <col min="2" max="2" width="18.28515625" customWidth="1"/>
     <col min="3" max="4" width="13.42578125" customWidth="1"/>
     <col min="5" max="5" width="40.42578125" customWidth="1"/>
+    <col min="6" max="6" width="5.7109375" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:10" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-    </row>
-    <row r="2" spans="1:5" ht="55.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+    </row>
+    <row r="2" spans="1:10" ht="55.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="D2" s="12" t="s">
-        <v>46</v>
+      <c r="C2" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>44</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="6">
@@ -1059,12 +1076,12 @@
         <v>43147</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="6">
@@ -1074,12 +1091,18 @@
         <v>43147</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+      <c r="G4" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="H4" s="16"/>
+      <c r="I4" s="16"/>
+      <c r="J4" s="16"/>
+    </row>
+    <row r="5" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="6">
@@ -1089,12 +1112,15 @@
         <v>43147</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+      <c r="G5" s="13">
+        <v>43088</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="6">
@@ -1104,28 +1130,35 @@
         <v>43147</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+      <c r="G6" s="13">
+        <v>43109</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B7" s="10"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
+        <v>45</v>
+      </c>
+      <c r="B7" s="8"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
       <c r="E7" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+      <c r="G7" s="13">
+        <v>43116</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="B8" s="3"/>
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>
-    </row>
-    <row r="9" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="G8" s="14"/>
+    </row>
+    <row r="9" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>34</v>
+        <v>53</v>
       </c>
       <c r="B9" s="3"/>
       <c r="C9" s="6">
@@ -1134,10 +1167,13 @@
       <c r="D9" s="6">
         <v>43147</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="G9" s="13">
+        <v>43123</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="6">
@@ -1146,10 +1182,13 @@
       <c r="D10" s="6">
         <v>43147</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="G10" s="13">
+        <v>43130</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B11" s="3"/>
       <c r="C11" s="6">
@@ -1158,10 +1197,13 @@
       <c r="D11" s="6">
         <v>43147</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="G11" s="13">
+        <v>43137</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>35</v>
+        <v>52</v>
       </c>
       <c r="B12" s="3"/>
       <c r="C12" s="6">
@@ -1170,35 +1212,44 @@
       <c r="D12" s="6">
         <v>43147</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" ht="37.5" x14ac:dyDescent="0.3">
+      <c r="G12" s="13">
+        <v>43144</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="6">
         <v>43089</v>
       </c>
       <c r="D13" s="6"/>
-      <c r="E13" s="9" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="E13" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="G13" s="13">
+        <v>43151</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B14" s="10"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="11"/>
-    </row>
-    <row r="15" spans="1:5" ht="18.75" hidden="1" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+      <c r="B14" s="8"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="G14" s="13">
+        <v>43158</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="18.75" hidden="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
       <c r="B15" s="3"/>
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
     </row>
-    <row r="16" spans="1:5" ht="18.75" hidden="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" ht="18.75" hidden="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
       <c r="B16" s="2"/>
       <c r="C16" s="6"/>
@@ -1206,7 +1257,7 @@
     </row>
     <row r="17" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B17" s="3"/>
       <c r="C17" s="6">
@@ -1218,7 +1269,7 @@
     </row>
     <row r="18" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B18" s="3"/>
       <c r="C18" s="6">
@@ -1230,7 +1281,7 @@
     </row>
     <row r="19" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B19" s="3"/>
       <c r="C19" s="6">
@@ -1242,7 +1293,7 @@
     </row>
     <row r="20" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B20" s="3"/>
       <c r="C20" s="6">

</xml_diff>

<commit_message>
Updated Task Assignment List 12Dec17
Assigned tasks to each team member
</commit_message>
<xml_diff>
--- a/Task Assignment List.xlsx
+++ b/Task Assignment List.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="55">
   <si>
     <t>Task</t>
   </si>
@@ -383,16 +383,16 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -739,12 +739,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
     </row>
     <row r="2" spans="1:4" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
@@ -905,12 +905,12 @@
       <c r="C17" s="6"/>
     </row>
     <row r="18" spans="1:4" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="11" t="s">
+      <c r="A18" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="B18" s="11"/>
-      <c r="C18" s="11"/>
-      <c r="D18" s="11"/>
+      <c r="B18" s="15"/>
+      <c r="C18" s="15"/>
+      <c r="D18" s="15"/>
     </row>
     <row r="19" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
@@ -1025,7 +1025,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I13" sqref="I13"/>
+      <selection pane="bottomLeft" activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1038,16 +1038,16 @@
     <col min="7" max="7" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-    </row>
-    <row r="2" spans="1:10" ht="55.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+    </row>
+    <row r="2" spans="1:10" ht="54.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>46</v>
       </c>
@@ -1068,7 +1068,9 @@
       <c r="A3" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B3" s="3"/>
+      <c r="B3" s="3" t="s">
+        <v>24</v>
+      </c>
       <c r="C3" s="6">
         <v>43119</v>
       </c>
@@ -1083,7 +1085,9 @@
       <c r="A4" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B4" s="3"/>
+      <c r="B4" s="3" t="s">
+        <v>24</v>
+      </c>
       <c r="C4" s="6">
         <v>43119</v>
       </c>
@@ -1093,18 +1097,20 @@
       <c r="E4" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="G4" s="15" t="s">
+      <c r="G4" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="H4" s="16"/>
-      <c r="I4" s="16"/>
-      <c r="J4" s="16"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="14"/>
+      <c r="J4" s="14"/>
     </row>
     <row r="5" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B5" s="3"/>
+      <c r="B5" s="3" t="s">
+        <v>25</v>
+      </c>
       <c r="C5" s="6">
         <v>43119</v>
       </c>
@@ -1114,7 +1120,7 @@
       <c r="E5" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="G5" s="13">
+      <c r="G5" s="11">
         <v>43088</v>
       </c>
     </row>
@@ -1122,7 +1128,9 @@
       <c r="A6" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B6" s="3"/>
+      <c r="B6" s="3" t="s">
+        <v>26</v>
+      </c>
       <c r="C6" s="6">
         <v>43119</v>
       </c>
@@ -1132,7 +1140,7 @@
       <c r="E6" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="G6" s="13">
+      <c r="G6" s="11">
         <v>43109</v>
       </c>
     </row>
@@ -1146,7 +1154,7 @@
       <c r="E7" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="G7" s="13">
+      <c r="G7" s="11">
         <v>43116</v>
       </c>
     </row>
@@ -1154,20 +1162,22 @@
       <c r="B8" s="3"/>
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>
-      <c r="G8" s="14"/>
+      <c r="G8" s="12"/>
     </row>
     <row r="9" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B9" s="3"/>
+      <c r="B9" s="3" t="s">
+        <v>23</v>
+      </c>
       <c r="C9" s="6">
         <v>43119</v>
       </c>
       <c r="D9" s="6">
         <v>43147</v>
       </c>
-      <c r="G9" s="13">
+      <c r="G9" s="11">
         <v>43123</v>
       </c>
     </row>
@@ -1175,14 +1185,16 @@
       <c r="A10" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B10" s="3"/>
+      <c r="B10" s="3" t="s">
+        <v>23</v>
+      </c>
       <c r="C10" s="6">
         <v>43119</v>
       </c>
       <c r="D10" s="6">
         <v>43147</v>
       </c>
-      <c r="G10" s="13">
+      <c r="G10" s="11">
         <v>43130</v>
       </c>
     </row>
@@ -1190,14 +1202,16 @@
       <c r="A11" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B11" s="3"/>
+      <c r="B11" s="3" t="s">
+        <v>14</v>
+      </c>
       <c r="C11" s="6">
         <v>43119</v>
       </c>
       <c r="D11" s="6">
         <v>43147</v>
       </c>
-      <c r="G11" s="13">
+      <c r="G11" s="11">
         <v>43137</v>
       </c>
     </row>
@@ -1205,14 +1219,16 @@
       <c r="A12" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B12" s="3"/>
+      <c r="B12" s="3" t="s">
+        <v>25</v>
+      </c>
       <c r="C12" s="6">
         <v>43119</v>
       </c>
       <c r="D12" s="6">
         <v>43147</v>
       </c>
-      <c r="G12" s="13">
+      <c r="G12" s="11">
         <v>43144</v>
       </c>
     </row>
@@ -1220,7 +1236,9 @@
       <c r="A13" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B13" s="2"/>
+      <c r="B13" s="3" t="s">
+        <v>14</v>
+      </c>
       <c r="C13" s="6">
         <v>43089</v>
       </c>
@@ -1228,7 +1246,7 @@
       <c r="E13" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="G13" s="13">
+      <c r="G13" s="11">
         <v>43151</v>
       </c>
     </row>
@@ -1239,7 +1257,7 @@
       <c r="B14" s="8"/>
       <c r="C14" s="9"/>
       <c r="D14" s="9"/>
-      <c r="G14" s="13">
+      <c r="G14" s="11">
         <v>43158</v>
       </c>
     </row>

</xml_diff>